<commit_message>
Added CP05MOAS-GL eng bar codes, corrected a couple reference designators
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP05MOAS-GL335_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_CP05MOAS-GL335_00001.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>Ref Des</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>CC_bsipar_par_scaling</t>
+  </si>
+  <si>
+    <t>OL000347</t>
   </si>
 </sst>
 </file>
@@ -770,7 +773,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +896,7 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,10 +1126,11 @@
         <v>124</v>
       </c>
       <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="J7" s="15"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
+      <c r="O7" s="15"/>
     </row>
     <row r="8" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1154,7 +1158,7 @@
         <v>700</v>
       </c>
       <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -1185,7 +1189,7 @@
         <v>1.0760000000000001</v>
       </c>
       <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="J9" s="15"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
@@ -1216,7 +1220,7 @@
         <v>3.9E-2</v>
       </c>
       <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
@@ -1231,7 +1235,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="19"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
+      <c r="J11" s="15"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
@@ -1258,7 +1262,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="11"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+      <c r="J12" s="15"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
@@ -1273,7 +1277,7 @@
       <c r="G13" s="10"/>
       <c r="H13" s="11"/>
       <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="J13" s="15"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
@@ -1300,7 +1304,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="11"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+      <c r="J14" s="15"/>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
@@ -1315,7 +1319,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="11"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="J15" s="15"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
@@ -1346,7 +1350,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
+      <c r="J16" s="15"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
@@ -1361,7 +1365,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="11"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
+      <c r="J17" s="15"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
@@ -1379,14 +1383,16 @@
       <c r="D18" s="12">
         <v>1</v>
       </c>
-      <c r="E18" s="12"/>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
       <c r="F18" s="16">
         <v>335</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="11"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
+      <c r="J18" s="15"/>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>

</xml_diff>